<commit_message>
Data Driven Approach applied in US_Gear05_Data Driven
</commit_message>
<xml_diff>
--- a/Resources/Datastore.xlsx
+++ b/Resources/Datastore.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
   <si>
     <t>Customer</t>
   </si>
@@ -133,16 +133,44 @@
   </si>
   <si>
     <t>Acushnet#1</t>
+  </si>
+  <si>
+    <t>customerNumber</t>
+  </si>
+  <si>
+    <t>coType</t>
+  </si>
+  <si>
+    <t>US00025065</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>US-Gear-06</t>
+  </si>
+  <si>
+    <t>ItemCode</t>
+  </si>
+  <si>
+    <t>TB7SX6CC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -168,8 +196,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -617,7 +646,7 @@
   <dimension ref="A1:V1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -709,31 +738,60 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B1" t="s">
         <v>37</v>
       </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>36</v>
       </c>
       <c r="B2" t="s">
         <v>38</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
format of cell in excel to string type
</commit_message>
<xml_diff>
--- a/Resources/Datastore.xlsx
+++ b/Resources/Datastore.xlsx
@@ -196,9 +196,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -741,13 +742,15 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -783,10 +786,10 @@
       <c r="D2" t="s">
         <v>42</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>

<commit_message>
change script 1 data to run on AGSAuto account instead of ajenkins
</commit_message>
<xml_diff>
--- a/Resources/Datastore.xlsx
+++ b/Resources/Datastore.xlsx
@@ -126,15 +126,9 @@
     <t>Username</t>
   </si>
   <si>
-    <t>ajenkins</t>
-  </si>
-  <si>
     <t>password</t>
   </si>
   <si>
-    <t>Acushnet#1</t>
-  </si>
-  <si>
     <t>customerNumber</t>
   </si>
   <si>
@@ -154,6 +148,12 @@
   </si>
   <si>
     <t>TB7SX6CC</t>
+  </si>
+  <si>
+    <t>AGSAutoT02</t>
+  </si>
+  <si>
+    <t>SERVICE$08</t>
   </si>
 </sst>
 </file>
@@ -742,15 +742,17 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -758,39 +760,39 @@
         <v>35</v>
       </c>
       <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
         <v>37</v>
       </c>
-      <c r="C1" t="s">
-        <v>39</v>
-      </c>
       <c r="D1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add function for entering item quantity
includes quantity value in excel
</commit_message>
<xml_diff>
--- a/Resources/Datastore.xlsx
+++ b/Resources/Datastore.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
   <si>
     <t>Customer</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>SERVICE$08</t>
+  </si>
+  <si>
+    <t>Quantity</t>
   </si>
 </sst>
 </file>
@@ -739,10 +742,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -755,7 +758,7 @@
     <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>35</v>
       </c>
@@ -774,8 +777,11 @@
       <c r="F1" t="s">
         <v>42</v>
       </c>
+      <c r="G1" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -793,6 +799,9 @@
       </c>
       <c r="F2" s="2" t="s">
         <v>43</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1-update datastore with new customer number
the other customer numbers were resulting in a credit hold on the orders, found one that doesn't do that. also, removing a line I accidentally submitted.
</commit_message>
<xml_diff>
--- a/Resources/Datastore.xlsx
+++ b/Resources/Datastore.xlsx
@@ -135,9 +135,6 @@
     <t>coType</t>
   </si>
   <si>
-    <t>US00025065</t>
-  </si>
-  <si>
     <t>USA</t>
   </si>
   <si>
@@ -157,13 +154,16 @@
   </si>
   <si>
     <t>Quantity</t>
+  </si>
+  <si>
+    <t>US00000571</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -174,6 +174,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -199,10 +206,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -745,7 +753,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,30 +783,30 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
         <v>44</v>
       </c>
-      <c r="B2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" t="s">
         <v>39</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="F2" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G2">
         <v>1</v>

</xml_diff>

<commit_message>
1-update configuration for new panel settings
</commit_message>
<xml_diff>
--- a/Resources/Datastore.xlsx
+++ b/Resources/Datastore.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
   <si>
     <t>Customer</t>
   </si>
@@ -144,19 +144,22 @@
     <t>ItemCode</t>
   </si>
   <si>
+    <t>AGSAutoT02</t>
+  </si>
+  <si>
+    <t>SERVICE$08</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>US00000571</t>
+  </si>
+  <si>
+    <t>TB7SX1CC</t>
+  </si>
+  <si>
     <t>TB7SX6CC</t>
-  </si>
-  <si>
-    <t>AGSAutoT02</t>
-  </si>
-  <si>
-    <t>SERVICE$08</t>
-  </si>
-  <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>US00000571</t>
   </si>
 </sst>
 </file>
@@ -750,10 +753,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -786,18 +789,18 @@
         <v>41</v>
       </c>
       <c r="G1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
         <v>43</v>
       </c>
-      <c r="B2" t="s">
-        <v>44</v>
-      </c>
       <c r="C2" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D2" t="s">
         <v>39</v>
@@ -806,10 +809,15 @@
         <v>40</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G2">
         <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F3" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed Item code to read from excel, from the 2nd row
</commit_message>
<xml_diff>
--- a/Resources/Datastore.xlsx
+++ b/Resources/Datastore.xlsx
@@ -166,7 +166,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -175,15 +175,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -197,7 +206,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -205,15 +214,93 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -756,7 +843,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -769,56 +856,62 @@
     <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="8" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
       <c r="F3" s="2" t="s">
         <v>46</v>
       </c>
+      <c r="G3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added login credentialsfor script 2 in Excel.
The idea is to maintain all log ins in one excel sheet, in different rows.
</commit_message>
<xml_diff>
--- a/Resources/Datastore.xlsx
+++ b/Resources/Datastore.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="50">
   <si>
     <t>Customer</t>
   </si>
@@ -157,13 +157,22 @@
   </si>
   <si>
     <t>Quantity</t>
+  </si>
+  <si>
+    <t>Script2</t>
+  </si>
+  <si>
+    <t>AGSAutoT03</t>
+  </si>
+  <si>
+    <t>TB7SX1CC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,6 +181,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -179,15 +197,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -195,14 +219,93 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -742,10 +845,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -758,49 +861,111 @@
     <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="8" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G12" s="4">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added login credentials for script 2 in excel
</commit_message>
<xml_diff>
--- a/Resources/Datastore.xlsx
+++ b/Resources/Datastore.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="90" windowWidth="20580" windowHeight="11640" activeTab="2"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="50">
   <si>
     <t>Customer</t>
   </si>
@@ -160,6 +160,12 @@
   </si>
   <si>
     <t>TB7SX6CC</t>
+  </si>
+  <si>
+    <t>Script 2</t>
+  </si>
+  <si>
+    <t>AGSAutoT03</t>
   </si>
 </sst>
 </file>
@@ -198,12 +204,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="6">
@@ -291,7 +303,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -301,6 +313,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -840,10 +853,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -913,6 +926,68 @@
       </c>
       <c r="G3" s="1"/>
     </row>
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G12" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G13" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update excel schedule number counter and 1-item number
</commit_message>
<xml_diff>
--- a/Resources/Datastore.xlsx
+++ b/Resources/Datastore.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
   <si>
     <t>Customer</t>
   </si>
@@ -753,7 +753,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -809,7 +809,7 @@
         <v>40</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -818,6 +818,11 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F3" s="2" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F4" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>